<commit_message>
chore(maintenance): update version and enhance maintenance data export
- Bump version from 1.4.0 to 1.5.0
- Expand export columns with maintenance interval, reminder, next date, and status fields
- Write record count to sheet cell D2
- Remove temporary maintenance_data.xlsx file after successful email sending
- Add error handling and logging for file deletion operations
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5310" windowHeight="660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5310" windowHeight="660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ПК АСУ ТП" sheetId="1" r:id="rId1"/>
@@ -22,20 +22,15 @@
     <definedName name="_FD2" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$H$270</definedName>
     <definedName name="_FilterDatabase" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$G$63</definedName>
     <definedName name="_FilterDatabase" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$H$270</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$G$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$G$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$K$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$K$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>№</t>
   </si>
@@ -46,9 +41,6 @@
     <t>Наименование</t>
   </si>
   <si>
-    <t>Обозначение ПК</t>
-  </si>
-  <si>
     <t>Место расположения</t>
   </si>
   <si>
@@ -73,10 +65,64 @@
     <t>DATA</t>
   </si>
   <si>
-    <t xml:space="preserve">Требуентся обслужить ПК на </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Требуентся обслужить ШКАФЫ на </t>
+    <t xml:space="preserve">Требуется обслужить ПК на </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требуется обслужить ШКАФЫ на </t>
+  </si>
+  <si>
+    <t>Интервал ТО (дней)</t>
+  </si>
+  <si>
+    <t>Напоминание (за дней)</t>
+  </si>
+  <si>
+    <t>Дата следующего ТО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус </t>
+  </si>
+  <si>
+    <t>ЗИФ-1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>05.09.2025</t>
+  </si>
+  <si>
+    <t>ОБСЛУЖИТЬ</t>
+  </si>
+  <si>
+    <t>Trassir Сервер</t>
+  </si>
+  <si>
+    <t>ZIF-1-Trassir-1</t>
+  </si>
+  <si>
+    <t>Серверная АСУТП (флотация)</t>
+  </si>
+  <si>
+    <t>Продуть от пыли</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>05.08.2025</t>
+  </si>
+  <si>
+    <t>{DATA}</t>
+  </si>
+  <si>
+    <t>{col}</t>
+  </si>
+  <si>
+    <t>Колличество:</t>
   </si>
 </sst>
 </file>
@@ -88,7 +134,7 @@
     <numFmt numFmtId="165" formatCode="#,##0&quot;р.&quot;;[Red]\-#,##0&quot;р.&quot;"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,14 +201,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,6 +217,39 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -204,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -331,53 +402,120 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39936521500289923"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyProtection="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
@@ -386,43 +524,149 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="10" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="23" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="13" xfId="22" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="22" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="21" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="21" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="23" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="41">
     <cellStyle name="Background" xfId="1"/>
+    <cellStyle name="Background 2" xfId="24"/>
     <cellStyle name="Card" xfId="2"/>
+    <cellStyle name="Card 2" xfId="25"/>
     <cellStyle name="Card B" xfId="3"/>
+    <cellStyle name="Card B 2" xfId="26"/>
     <cellStyle name="Card BL" xfId="4"/>
+    <cellStyle name="Card BL 2" xfId="27"/>
     <cellStyle name="Card BR" xfId="5"/>
+    <cellStyle name="Card BR 2" xfId="28"/>
     <cellStyle name="Card L" xfId="6"/>
+    <cellStyle name="Card L 2" xfId="29"/>
     <cellStyle name="Card R" xfId="7"/>
+    <cellStyle name="Card R 2" xfId="30"/>
     <cellStyle name="Card T" xfId="8"/>
+    <cellStyle name="Card T 2" xfId="31"/>
     <cellStyle name="Card TL" xfId="9"/>
+    <cellStyle name="Card TL 2" xfId="32"/>
     <cellStyle name="Card TR" xfId="10"/>
+    <cellStyle name="Card TR 2" xfId="33"/>
     <cellStyle name="Column Header" xfId="11"/>
+    <cellStyle name="Column Header 2" xfId="34"/>
     <cellStyle name="Excel Built-in Heading 3" xfId="20"/>
+    <cellStyle name="Excel Built-in Heading 3 2" xfId="40"/>
     <cellStyle name="Excel Built-in Heading 4" xfId="19"/>
+    <cellStyle name="Excel Built-in Heading 4 2" xfId="39"/>
     <cellStyle name="Heading 1 1" xfId="12"/>
+    <cellStyle name="Heading 1 1 2" xfId="35"/>
     <cellStyle name="Heading 2 2" xfId="13"/>
+    <cellStyle name="Heading 2 2 2" xfId="36"/>
     <cellStyle name="Input" xfId="14"/>
     <cellStyle name="Red BG" xfId="15"/>
+    <cellStyle name="Red BG 2" xfId="37"/>
+    <cellStyle name="Заголовок 1" xfId="21" builtinId="16"/>
+    <cellStyle name="Заголовок 2" xfId="22" builtinId="17"/>
+    <cellStyle name="Заголовок 4" xfId="23" builtinId="19"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="16"/>
     <cellStyle name="Обычный 3" xfId="17"/>
     <cellStyle name="Результат2" xfId="18"/>
+    <cellStyle name="Результат2 2" xfId="38"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF006600"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF996600"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFCC0000"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF006600"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF996600"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFCC0000"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -501,6 +745,104 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>55563</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>706782</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>167032</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14803438" y="55563"/>
+          <a:ext cx="579782" cy="579782"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>124240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>704022</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16739153" y="33130"/>
+          <a:ext cx="579782" cy="579782"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -684,139 +1026,200 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:G4"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="56.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="17" t="s">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G5" s="13"/>
+      <c r="J4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G6" s="13"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D7" s="14"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D8" s="14"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="11"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="14"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G10" s="13"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G11" s="13"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G12" s="13"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G13" s="13"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G14" s="13"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G15" s="13"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="13"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="13"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="13"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="14"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="11"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="14"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="11"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="13"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="13"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="16"/>
+      <c r="E32" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G4"/>
+  <autoFilter ref="A4:K4"/>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"ОБСЛУЖИТЬ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Внимание"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Не требуется"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="49" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -825,360 +1228,424 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H233"/>
+  <dimension ref="A1:K233"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="31.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="61.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="17" t="s">
-        <v>11</v>
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="C2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G13" s="13"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G16" s="13"/>
+      <c r="J4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="13"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="13"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="13"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="13"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="13"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="13"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="13"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="13"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="13"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="13"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="13"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="13"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="13"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="13"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52" s="13"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53" s="13"/>
+      <c r="G53" s="10"/>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="13"/>
+      <c r="G54" s="10"/>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="13"/>
+      <c r="G55" s="10"/>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G56" s="13"/>
+      <c r="G56" s="10"/>
     </row>
     <row r="57" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G57" s="13"/>
+      <c r="G57" s="10"/>
     </row>
     <row r="60" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G60" s="13"/>
+      <c r="G60" s="10"/>
     </row>
     <row r="61" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G61" s="13"/>
+      <c r="G61" s="10"/>
     </row>
     <row r="62" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G62" s="13"/>
+      <c r="G62" s="10"/>
     </row>
     <row r="63" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G63" s="13"/>
+      <c r="G63" s="10"/>
     </row>
     <row r="64" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G64" s="13"/>
+      <c r="G64" s="10"/>
     </row>
     <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65" s="13"/>
+      <c r="G65" s="10"/>
     </row>
     <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66" s="13"/>
+      <c r="G66" s="10"/>
     </row>
     <row r="67" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G67" s="13"/>
+      <c r="G67" s="10"/>
     </row>
     <row r="68" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G68" s="13"/>
+      <c r="G68" s="10"/>
     </row>
     <row r="69" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G69" s="13"/>
+      <c r="G69" s="10"/>
     </row>
     <row r="70" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G70" s="13"/>
+      <c r="G70" s="10"/>
     </row>
     <row r="71" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G71" s="13"/>
+      <c r="G71" s="10"/>
     </row>
     <row r="72" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G72" s="13"/>
+      <c r="G72" s="10"/>
     </row>
     <row r="73" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G73" s="13"/>
+      <c r="G73" s="10"/>
     </row>
     <row r="74" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G74" s="13"/>
+      <c r="G74" s="10"/>
     </row>
     <row r="75" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G75" s="13"/>
+      <c r="G75" s="10"/>
     </row>
     <row r="76" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G76" s="13"/>
+      <c r="G76" s="10"/>
     </row>
     <row r="77" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G77" s="13"/>
+      <c r="G77" s="10"/>
     </row>
     <row r="78" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G78" s="13"/>
+      <c r="G78" s="10"/>
     </row>
     <row r="79" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G79" s="13"/>
+      <c r="G79" s="10"/>
     </row>
     <row r="80" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G80" s="13"/>
+      <c r="G80" s="10"/>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G81" s="13"/>
+      <c r="G81" s="10"/>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G82" s="13"/>
+      <c r="G82" s="10"/>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83" s="13"/>
+      <c r="G83" s="10"/>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84" s="13"/>
+      <c r="G84" s="10"/>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85" s="13"/>
+      <c r="G85" s="10"/>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G92" s="13"/>
+      <c r="G92" s="10"/>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G94" s="13"/>
+      <c r="G94" s="10"/>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G95" s="13"/>
+      <c r="G95" s="10"/>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G97" s="13"/>
+      <c r="G97" s="10"/>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G98" s="13"/>
+      <c r="G98" s="10"/>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G99" s="13"/>
+      <c r="G99" s="10"/>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G100" s="13"/>
+      <c r="G100" s="10"/>
     </row>
     <row r="103" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G103" s="13"/>
+      <c r="G103" s="10"/>
     </row>
     <row r="118" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D118" s="16"/>
+      <c r="D118" s="13"/>
     </row>
     <row r="123" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G123" s="13"/>
+      <c r="G123" s="10"/>
     </row>
     <row r="124" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G124" s="13"/>
+      <c r="G124" s="10"/>
     </row>
     <row r="125" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G125" s="13"/>
+      <c r="G125" s="10"/>
     </row>
     <row r="126" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G126" s="13"/>
+      <c r="G126" s="10"/>
     </row>
     <row r="138" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G138" s="13"/>
+      <c r="G138" s="10"/>
     </row>
     <row r="146" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G146" s="13"/>
+      <c r="G146" s="10"/>
     </row>
     <row r="153" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G153" s="13"/>
+      <c r="G153" s="10"/>
     </row>
     <row r="186" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G186" s="13"/>
+      <c r="G186" s="10"/>
     </row>
     <row r="187" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G187" s="13"/>
+      <c r="G187" s="10"/>
     </row>
     <row r="205" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G205" s="13"/>
+      <c r="G205" s="10"/>
     </row>
     <row r="207" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G207" s="13"/>
+      <c r="G207" s="10"/>
     </row>
     <row r="209" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G209" s="13"/>
+      <c r="G209" s="10"/>
     </row>
     <row r="215" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G215" s="13"/>
+      <c r="G215" s="10"/>
     </row>
     <row r="216" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G216" s="13"/>
+      <c r="G216" s="10"/>
     </row>
     <row r="217" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G217" s="13"/>
+      <c r="G217" s="10"/>
     </row>
     <row r="218" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G218" s="13"/>
+      <c r="G218" s="10"/>
     </row>
     <row r="219" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G219" s="13"/>
+      <c r="G219" s="10"/>
     </row>
     <row r="220" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G220" s="13"/>
+      <c r="G220" s="10"/>
     </row>
     <row r="221" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G221" s="13"/>
+      <c r="G221" s="10"/>
     </row>
     <row r="225" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G225" s="13"/>
+      <c r="G225" s="10"/>
     </row>
     <row r="226" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G226" s="13"/>
+      <c r="G226" s="10"/>
     </row>
     <row r="227" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G227" s="13"/>
+      <c r="G227" s="10"/>
     </row>
     <row r="228" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G228" s="13"/>
+      <c r="G228" s="10"/>
     </row>
     <row r="229" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G229" s="13"/>
+      <c r="G229" s="10"/>
     </row>
     <row r="230" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G230" s="13"/>
+      <c r="G230" s="10"/>
     </row>
     <row r="231" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G231" s="13"/>
+      <c r="G231" s="10"/>
     </row>
     <row r="232" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G232" s="13"/>
+      <c r="G232" s="10"/>
     </row>
     <row r="233" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G233" s="13"/>
+      <c r="G233" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G4"/>
+  <autoFilter ref="A4:K4"/>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"ОБСЛУЖИТЬ"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Внимание"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Не требуется"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="43" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1197,17 +1664,17 @@
   <sheetData>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>